<commit_message>
GAMS and Pyomo produces same results
</commit_message>
<xml_diff>
--- a/Borouge_Data_Scott_Demo.xlsx
+++ b/Borouge_Data_Scott_Demo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8955" firstSheet="7" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8955" firstSheet="7" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1194" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1199" uniqueCount="264">
   <si>
     <t>dim</t>
   </si>
@@ -1428,21 +1428,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1460,6 +1445,21 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2446,13 +2446,13 @@
   </sheetPr>
   <dimension ref="A1:O57"/>
   <sheetViews>
-    <sheetView showZeros="0" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView showZeros="0" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="S46" sqref="S46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="4.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.5703125" customWidth="1"/>
   </cols>
@@ -4099,7 +4099,7 @@
   <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView showZeros="0" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4385,7 +4385,7 @@
   <dimension ref="B1:N30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J30" sqref="J30:J31"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4857,8 +4857,8 @@
   </sheetPr>
   <dimension ref="A1:R175"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q32" sqref="Q32"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="I150" sqref="I150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4984,10 +4984,10 @@
       </c>
     </row>
     <row r="8" spans="2:18" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="116" t="s">
+      <c r="B8" s="124" t="s">
         <v>183</v>
       </c>
-      <c r="C8" s="117" t="s">
+      <c r="C8" s="125" t="s">
         <v>229</v>
       </c>
       <c r="D8" s="74" t="s">
@@ -5023,8 +5023,8 @@
       <c r="R8" s="49"/>
     </row>
     <row r="9" spans="2:18" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="116"/>
-      <c r="C9" s="118"/>
+      <c r="B9" s="124"/>
+      <c r="C9" s="126"/>
       <c r="D9" s="74" t="s">
         <v>246</v>
       </c>
@@ -5057,8 +5057,8 @@
       <c r="Q9" s="49"/>
     </row>
     <row r="10" spans="2:18" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="116"/>
-      <c r="C10" s="118"/>
+      <c r="B10" s="124"/>
+      <c r="C10" s="126"/>
       <c r="D10" s="74" t="s">
         <v>246</v>
       </c>
@@ -5091,8 +5091,8 @@
       <c r="Q10" s="49"/>
     </row>
     <row r="11" spans="2:18" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="116"/>
-      <c r="C11" s="118"/>
+      <c r="B11" s="124"/>
+      <c r="C11" s="126"/>
       <c r="D11" s="74" t="s">
         <v>246</v>
       </c>
@@ -5125,8 +5125,8 @@
       <c r="Q11" s="49"/>
     </row>
     <row r="12" spans="2:18" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="116"/>
-      <c r="C12" s="118"/>
+      <c r="B12" s="124"/>
+      <c r="C12" s="126"/>
       <c r="D12" s="74" t="s">
         <v>246</v>
       </c>
@@ -5159,8 +5159,8 @@
       <c r="Q12" s="49"/>
     </row>
     <row r="13" spans="2:18" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="116"/>
-      <c r="C13" s="118"/>
+      <c r="B13" s="124"/>
+      <c r="C13" s="126"/>
       <c r="D13" s="74" t="s">
         <v>246</v>
       </c>
@@ -5193,8 +5193,8 @@
       <c r="Q13" s="49"/>
     </row>
     <row r="14" spans="2:18" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="116"/>
-      <c r="C14" s="118"/>
+      <c r="B14" s="124"/>
+      <c r="C14" s="126"/>
       <c r="D14" s="74" t="s">
         <v>246</v>
       </c>
@@ -5227,8 +5227,8 @@
       <c r="Q14" s="49"/>
     </row>
     <row r="15" spans="2:18" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="116"/>
-      <c r="C15" s="118"/>
+      <c r="B15" s="124"/>
+      <c r="C15" s="126"/>
       <c r="D15" s="74" t="s">
         <v>246</v>
       </c>
@@ -5261,8 +5261,8 @@
       <c r="Q15" s="49"/>
     </row>
     <row r="16" spans="2:18" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="116"/>
-      <c r="C16" s="118"/>
+      <c r="B16" s="124"/>
+      <c r="C16" s="126"/>
       <c r="D16" s="74" t="s">
         <v>246</v>
       </c>
@@ -5295,8 +5295,8 @@
       <c r="Q16" s="49"/>
     </row>
     <row r="17" spans="2:17" s="50" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="116"/>
-      <c r="C17" s="118"/>
+      <c r="B17" s="124"/>
+      <c r="C17" s="126"/>
       <c r="D17" s="74" t="s">
         <v>246</v>
       </c>
@@ -5360,10 +5360,10 @@
       <c r="N18" s="49"/>
     </row>
     <row r="19" spans="2:17" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="116" t="s">
+      <c r="B19" s="124" t="s">
         <v>222</v>
       </c>
-      <c r="C19" s="117" t="s">
+      <c r="C19" s="125" t="s">
         <v>229</v>
       </c>
       <c r="D19" s="74" t="s">
@@ -5395,8 +5395,8 @@
       <c r="N19" s="49"/>
     </row>
     <row r="20" spans="2:17" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="116"/>
-      <c r="C20" s="118"/>
+      <c r="B20" s="124"/>
+      <c r="C20" s="126"/>
       <c r="D20" s="74" t="s">
         <v>241</v>
       </c>
@@ -5426,8 +5426,8 @@
       <c r="N20" s="49"/>
     </row>
     <row r="21" spans="2:17" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="116"/>
-      <c r="C21" s="118"/>
+      <c r="B21" s="124"/>
+      <c r="C21" s="126"/>
       <c r="D21" s="74" t="s">
         <v>241</v>
       </c>
@@ -5457,8 +5457,8 @@
       <c r="N21" s="49"/>
     </row>
     <row r="22" spans="2:17" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="116"/>
-      <c r="C22" s="118"/>
+      <c r="B22" s="124"/>
+      <c r="C22" s="126"/>
       <c r="D22" s="74" t="s">
         <v>241</v>
       </c>
@@ -5488,8 +5488,8 @@
       <c r="N22" s="49"/>
     </row>
     <row r="23" spans="2:17" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="116"/>
-      <c r="C23" s="118"/>
+      <c r="B23" s="124"/>
+      <c r="C23" s="126"/>
       <c r="D23" s="74" t="s">
         <v>241</v>
       </c>
@@ -5519,8 +5519,8 @@
       <c r="N23" s="49"/>
     </row>
     <row r="24" spans="2:17" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="116"/>
-      <c r="C24" s="118"/>
+      <c r="B24" s="124"/>
+      <c r="C24" s="126"/>
       <c r="D24" s="74" t="s">
         <v>241</v>
       </c>
@@ -5550,8 +5550,8 @@
       <c r="N24" s="49"/>
     </row>
     <row r="25" spans="2:17" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="116"/>
-      <c r="C25" s="118"/>
+      <c r="B25" s="124"/>
+      <c r="C25" s="126"/>
       <c r="D25" s="74" t="s">
         <v>241</v>
       </c>
@@ -5581,8 +5581,8 @@
       <c r="N25" s="49"/>
     </row>
     <row r="26" spans="2:17" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="116"/>
-      <c r="C26" s="118"/>
+      <c r="B26" s="124"/>
+      <c r="C26" s="126"/>
       <c r="D26" s="74" t="s">
         <v>241</v>
       </c>
@@ -5612,8 +5612,8 @@
       <c r="N26" s="49"/>
     </row>
     <row r="27" spans="2:17" s="50" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="116"/>
-      <c r="C27" s="118"/>
+      <c r="B27" s="124"/>
+      <c r="C27" s="126"/>
       <c r="D27" s="74" t="s">
         <v>241</v>
       </c>
@@ -5643,8 +5643,8 @@
       <c r="N27" s="49"/>
     </row>
     <row r="28" spans="2:17" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="116"/>
-      <c r="C28" s="118"/>
+      <c r="B28" s="124"/>
+      <c r="C28" s="126"/>
       <c r="D28" s="74" t="s">
         <v>242</v>
       </c>
@@ -5702,10 +5702,10 @@
       </c>
     </row>
     <row r="30" spans="2:17" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="121" t="s">
+      <c r="B30" s="116" t="s">
         <v>184</v>
       </c>
-      <c r="C30" s="122" t="s">
+      <c r="C30" s="117" t="s">
         <v>229</v>
       </c>
       <c r="D30" s="74" t="s">
@@ -5737,8 +5737,8 @@
       <c r="N30" s="52"/>
     </row>
     <row r="31" spans="2:17" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="121"/>
-      <c r="C31" s="125"/>
+      <c r="B31" s="116"/>
+      <c r="C31" s="120"/>
       <c r="D31" s="74" t="s">
         <v>242</v>
       </c>
@@ -5768,8 +5768,8 @@
       <c r="N31" s="52"/>
     </row>
     <row r="32" spans="2:17" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="121"/>
-      <c r="C32" s="125"/>
+      <c r="B32" s="116"/>
+      <c r="C32" s="120"/>
       <c r="D32" s="74" t="s">
         <v>242</v>
       </c>
@@ -5799,8 +5799,8 @@
       <c r="N32" s="52"/>
     </row>
     <row r="33" spans="2:14" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="121"/>
-      <c r="C33" s="125"/>
+      <c r="B33" s="116"/>
+      <c r="C33" s="120"/>
       <c r="D33" s="74" t="s">
         <v>242</v>
       </c>
@@ -5830,8 +5830,8 @@
       <c r="N33" s="52"/>
     </row>
     <row r="34" spans="2:14" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="121"/>
-      <c r="C34" s="125"/>
+      <c r="B34" s="116"/>
+      <c r="C34" s="120"/>
       <c r="D34" s="74" t="s">
         <v>242</v>
       </c>
@@ -5861,8 +5861,8 @@
       <c r="N34" s="52"/>
     </row>
     <row r="35" spans="2:14" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="121"/>
-      <c r="C35" s="125"/>
+      <c r="B35" s="116"/>
+      <c r="C35" s="120"/>
       <c r="D35" s="74" t="s">
         <v>242</v>
       </c>
@@ -5892,8 +5892,8 @@
       <c r="N35" s="52"/>
     </row>
     <row r="36" spans="2:14" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="121"/>
-      <c r="C36" s="125"/>
+      <c r="B36" s="116"/>
+      <c r="C36" s="120"/>
       <c r="D36" s="74" t="s">
         <v>242</v>
       </c>
@@ -5923,8 +5923,8 @@
       <c r="N36" s="52"/>
     </row>
     <row r="37" spans="2:14" s="53" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="121"/>
-      <c r="C37" s="125"/>
+      <c r="B37" s="116"/>
+      <c r="C37" s="120"/>
       <c r="D37" s="74" t="s">
         <v>242</v>
       </c>
@@ -5954,8 +5954,8 @@
       <c r="N37" s="52"/>
     </row>
     <row r="38" spans="2:14" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="121"/>
-      <c r="C38" s="125"/>
+      <c r="B38" s="116"/>
+      <c r="C38" s="120"/>
       <c r="D38" s="74" t="s">
         <v>243</v>
       </c>
@@ -5985,8 +5985,8 @@
       <c r="N38" s="52"/>
     </row>
     <row r="39" spans="2:14" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="121"/>
-      <c r="C39" s="125"/>
+      <c r="B39" s="116"/>
+      <c r="C39" s="120"/>
       <c r="D39" s="74" t="s">
         <v>243</v>
       </c>
@@ -6047,10 +6047,10 @@
       <c r="N40" s="52"/>
     </row>
     <row r="41" spans="2:14" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="121" t="s">
+      <c r="B41" s="116" t="s">
         <v>221</v>
       </c>
-      <c r="C41" s="122" t="s">
+      <c r="C41" s="117" t="s">
         <v>229</v>
       </c>
       <c r="D41" s="74" t="s">
@@ -6082,8 +6082,8 @@
       <c r="N41" s="52"/>
     </row>
     <row r="42" spans="2:14" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="121"/>
-      <c r="C42" s="125"/>
+      <c r="B42" s="116"/>
+      <c r="C42" s="120"/>
       <c r="D42" s="74" t="s">
         <v>243</v>
       </c>
@@ -6113,8 +6113,8 @@
       <c r="N42" s="52"/>
     </row>
     <row r="43" spans="2:14" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="121"/>
-      <c r="C43" s="125"/>
+      <c r="B43" s="116"/>
+      <c r="C43" s="120"/>
       <c r="D43" s="74" t="s">
         <v>243</v>
       </c>
@@ -6144,8 +6144,8 @@
       <c r="N43" s="52"/>
     </row>
     <row r="44" spans="2:14" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="121"/>
-      <c r="C44" s="125"/>
+      <c r="B44" s="116"/>
+      <c r="C44" s="120"/>
       <c r="D44" s="74" t="s">
         <v>243</v>
       </c>
@@ -6175,8 +6175,8 @@
       <c r="N44" s="52"/>
     </row>
     <row r="45" spans="2:14" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="121"/>
-      <c r="C45" s="125"/>
+      <c r="B45" s="116"/>
+      <c r="C45" s="120"/>
       <c r="D45" s="74" t="s">
         <v>243</v>
       </c>
@@ -6206,8 +6206,8 @@
       <c r="N45" s="52"/>
     </row>
     <row r="46" spans="2:14" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="121"/>
-      <c r="C46" s="125"/>
+      <c r="B46" s="116"/>
+      <c r="C46" s="120"/>
       <c r="D46" s="74" t="s">
         <v>243</v>
       </c>
@@ -6237,8 +6237,8 @@
       <c r="N46" s="52"/>
     </row>
     <row r="47" spans="2:14" s="53" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="121"/>
-      <c r="C47" s="125"/>
+      <c r="B47" s="116"/>
+      <c r="C47" s="120"/>
       <c r="D47" s="74" t="s">
         <v>243</v>
       </c>
@@ -6268,8 +6268,8 @@
       <c r="N47" s="52"/>
     </row>
     <row r="48" spans="2:14" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="121"/>
-      <c r="C48" s="125"/>
+      <c r="B48" s="116"/>
+      <c r="C48" s="120"/>
       <c r="D48" s="74" t="s">
         <v>244</v>
       </c>
@@ -6299,8 +6299,8 @@
       <c r="N48" s="52"/>
     </row>
     <row r="49" spans="2:14" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="121"/>
-      <c r="C49" s="125"/>
+      <c r="B49" s="116"/>
+      <c r="C49" s="120"/>
       <c r="D49" s="74" t="s">
         <v>244</v>
       </c>
@@ -6330,8 +6330,8 @@
       <c r="N49" s="52"/>
     </row>
     <row r="50" spans="2:14" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="121"/>
-      <c r="C50" s="125"/>
+      <c r="B50" s="116"/>
+      <c r="C50" s="120"/>
       <c r="D50" s="74" t="s">
         <v>244</v>
       </c>
@@ -6389,10 +6389,10 @@
       </c>
     </row>
     <row r="52" spans="2:14" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="126" t="s">
+      <c r="B52" s="121" t="s">
         <v>185</v>
       </c>
-      <c r="C52" s="119" t="s">
+      <c r="C52" s="122" t="s">
         <v>229</v>
       </c>
       <c r="D52" s="74" t="s">
@@ -6421,8 +6421,8 @@
       </c>
     </row>
     <row r="53" spans="2:14" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="126"/>
-      <c r="C53" s="120"/>
+      <c r="B53" s="121"/>
+      <c r="C53" s="123"/>
       <c r="D53" s="74" t="s">
         <v>244</v>
       </c>
@@ -6449,8 +6449,8 @@
       </c>
     </row>
     <row r="54" spans="2:14" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="126"/>
-      <c r="C54" s="120"/>
+      <c r="B54" s="121"/>
+      <c r="C54" s="123"/>
       <c r="D54" s="74" t="s">
         <v>244</v>
       </c>
@@ -6477,8 +6477,8 @@
       </c>
     </row>
     <row r="55" spans="2:14" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="126"/>
-      <c r="C55" s="120"/>
+      <c r="B55" s="121"/>
+      <c r="C55" s="123"/>
       <c r="D55" s="74" t="s">
         <v>244</v>
       </c>
@@ -6505,8 +6505,8 @@
       </c>
     </row>
     <row r="56" spans="2:14" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="126"/>
-      <c r="C56" s="120"/>
+      <c r="B56" s="121"/>
+      <c r="C56" s="123"/>
       <c r="D56" s="74" t="s">
         <v>244</v>
       </c>
@@ -6533,8 +6533,8 @@
       </c>
     </row>
     <row r="57" spans="2:14" s="67" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="126"/>
-      <c r="C57" s="120"/>
+      <c r="B57" s="121"/>
+      <c r="C57" s="123"/>
       <c r="D57" s="74" t="s">
         <v>244</v>
       </c>
@@ -6561,8 +6561,8 @@
       </c>
     </row>
     <row r="58" spans="2:14" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="126"/>
-      <c r="C58" s="120"/>
+      <c r="B58" s="121"/>
+      <c r="C58" s="123"/>
       <c r="D58" s="74" t="s">
         <v>245</v>
       </c>
@@ -6589,8 +6589,8 @@
       </c>
     </row>
     <row r="59" spans="2:14" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="126"/>
-      <c r="C59" s="120"/>
+      <c r="B59" s="121"/>
+      <c r="C59" s="123"/>
       <c r="D59" s="74" t="s">
         <v>245</v>
       </c>
@@ -6617,8 +6617,8 @@
       </c>
     </row>
     <row r="60" spans="2:14" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="126"/>
-      <c r="C60" s="120"/>
+      <c r="B60" s="121"/>
+      <c r="C60" s="123"/>
       <c r="D60" s="74" t="s">
         <v>245</v>
       </c>
@@ -6645,8 +6645,8 @@
       </c>
     </row>
     <row r="61" spans="2:14" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="126"/>
-      <c r="C61" s="120"/>
+      <c r="B61" s="121"/>
+      <c r="C61" s="123"/>
       <c r="D61" s="74" t="s">
         <v>245</v>
       </c>
@@ -6700,8 +6700,8 @@
       </c>
     </row>
     <row r="63" spans="2:14" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="126"/>
-      <c r="C63" s="119"/>
+      <c r="B63" s="121"/>
+      <c r="C63" s="122"/>
       <c r="D63" s="74" t="s">
         <v>245</v>
       </c>
@@ -6728,8 +6728,8 @@
       </c>
     </row>
     <row r="64" spans="2:14" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="126"/>
-      <c r="C64" s="120"/>
+      <c r="B64" s="121"/>
+      <c r="C64" s="123"/>
       <c r="D64" s="74" t="s">
         <v>245</v>
       </c>
@@ -6756,8 +6756,8 @@
       </c>
     </row>
     <row r="65" spans="2:18" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="126"/>
-      <c r="C65" s="120"/>
+      <c r="B65" s="121"/>
+      <c r="C65" s="123"/>
       <c r="D65" s="74" t="s">
         <v>245</v>
       </c>
@@ -6784,8 +6784,8 @@
       </c>
     </row>
     <row r="66" spans="2:18" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="126"/>
-      <c r="C66" s="120"/>
+      <c r="B66" s="121"/>
+      <c r="C66" s="123"/>
       <c r="D66" s="74" t="s">
         <v>245</v>
       </c>
@@ -6812,8 +6812,8 @@
       </c>
     </row>
     <row r="67" spans="2:18" s="67" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="126"/>
-      <c r="C67" s="120"/>
+      <c r="B67" s="121"/>
+      <c r="C67" s="123"/>
       <c r="D67" s="74" t="s">
         <v>245</v>
       </c>
@@ -6840,24 +6840,24 @@
       </c>
     </row>
     <row r="68" spans="2:18" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="126"/>
-      <c r="C68" s="120"/>
+      <c r="B68" s="121"/>
+      <c r="C68" s="123"/>
     </row>
     <row r="69" spans="2:18" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="126"/>
-      <c r="C69" s="120"/>
+      <c r="B69" s="121"/>
+      <c r="C69" s="123"/>
     </row>
     <row r="70" spans="2:18" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="126"/>
-      <c r="C70" s="120"/>
+      <c r="B70" s="121"/>
+      <c r="C70" s="123"/>
     </row>
     <row r="71" spans="2:18" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="126"/>
-      <c r="C71" s="120"/>
+      <c r="B71" s="121"/>
+      <c r="C71" s="123"/>
     </row>
     <row r="72" spans="2:18" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="126"/>
-      <c r="C72" s="120"/>
+      <c r="B72" s="121"/>
+      <c r="C72" s="123"/>
     </row>
     <row r="73" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B73" s="9" t="s">
@@ -6891,10 +6891,10 @@
       </c>
     </row>
     <row r="75" spans="2:18" s="50" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="116" t="s">
+      <c r="B75" s="124" t="s">
         <v>223</v>
       </c>
-      <c r="C75" s="117" t="s">
+      <c r="C75" s="125" t="s">
         <v>232</v>
       </c>
       <c r="D75" s="74" t="s">
@@ -6930,8 +6930,8 @@
       <c r="R75" s="49"/>
     </row>
     <row r="76" spans="2:18" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="116"/>
-      <c r="C76" s="118"/>
+      <c r="B76" s="124"/>
+      <c r="C76" s="126"/>
       <c r="D76" s="74" t="s">
         <v>246</v>
       </c>
@@ -6965,8 +6965,8 @@
       <c r="R76" s="49"/>
     </row>
     <row r="77" spans="2:18" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="116"/>
-      <c r="C77" s="118"/>
+      <c r="B77" s="124"/>
+      <c r="C77" s="126"/>
       <c r="D77" s="74" t="s">
         <v>246</v>
       </c>
@@ -7000,8 +7000,8 @@
       <c r="R77" s="49"/>
     </row>
     <row r="78" spans="2:18" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="116"/>
-      <c r="C78" s="118"/>
+      <c r="B78" s="124"/>
+      <c r="C78" s="126"/>
       <c r="D78" s="74" t="s">
         <v>246</v>
       </c>
@@ -7035,8 +7035,8 @@
       <c r="R78" s="49"/>
     </row>
     <row r="79" spans="2:18" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="116"/>
-      <c r="C79" s="118"/>
+      <c r="B79" s="124"/>
+      <c r="C79" s="126"/>
       <c r="D79" s="74" t="s">
         <v>246</v>
       </c>
@@ -7070,8 +7070,8 @@
       <c r="R79" s="49"/>
     </row>
     <row r="80" spans="2:18" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="116"/>
-      <c r="C80" s="118"/>
+      <c r="B80" s="124"/>
+      <c r="C80" s="126"/>
       <c r="D80" s="74" t="s">
         <v>246</v>
       </c>
@@ -7105,8 +7105,8 @@
       <c r="R80" s="49"/>
     </row>
     <row r="81" spans="2:18" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B81" s="116"/>
-      <c r="C81" s="118"/>
+      <c r="B81" s="124"/>
+      <c r="C81" s="126"/>
       <c r="D81" s="74" t="s">
         <v>246</v>
       </c>
@@ -7140,8 +7140,8 @@
       <c r="R81" s="49"/>
     </row>
     <row r="82" spans="2:18" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="116"/>
-      <c r="C82" s="118"/>
+      <c r="B82" s="124"/>
+      <c r="C82" s="126"/>
       <c r="D82" s="74" t="s">
         <v>246</v>
       </c>
@@ -7175,8 +7175,8 @@
       <c r="R82" s="49"/>
     </row>
     <row r="83" spans="2:18" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="116"/>
-      <c r="C83" s="118"/>
+      <c r="B83" s="124"/>
+      <c r="C83" s="126"/>
       <c r="D83" s="74" t="s">
         <v>246</v>
       </c>
@@ -7210,8 +7210,8 @@
       <c r="R83" s="49"/>
     </row>
     <row r="84" spans="2:18" s="50" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B84" s="116"/>
-      <c r="C84" s="118"/>
+      <c r="B84" s="124"/>
+      <c r="C84" s="126"/>
       <c r="D84" s="74" t="s">
         <v>246</v>
       </c>
@@ -7278,10 +7278,10 @@
       </c>
     </row>
     <row r="86" spans="2:18" s="53" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B86" s="121" t="s">
+      <c r="B86" s="116" t="s">
         <v>175</v>
       </c>
-      <c r="C86" s="122" t="s">
+      <c r="C86" s="117" t="s">
         <v>232</v>
       </c>
       <c r="D86" s="74" t="s">
@@ -7319,8 +7319,8 @@
       <c r="N86" s="52"/>
     </row>
     <row r="87" spans="2:18" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="121"/>
-      <c r="C87" s="122"/>
+      <c r="B87" s="116"/>
+      <c r="C87" s="117"/>
       <c r="D87" s="74" t="s">
         <v>241</v>
       </c>
@@ -7356,8 +7356,8 @@
       <c r="N87" s="52"/>
     </row>
     <row r="88" spans="2:18" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="121"/>
-      <c r="C88" s="122"/>
+      <c r="B88" s="116"/>
+      <c r="C88" s="117"/>
       <c r="D88" s="74" t="s">
         <v>241</v>
       </c>
@@ -7393,8 +7393,8 @@
       <c r="N88" s="52"/>
     </row>
     <row r="89" spans="2:18" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B89" s="121"/>
-      <c r="C89" s="122"/>
+      <c r="B89" s="116"/>
+      <c r="C89" s="117"/>
       <c r="D89" s="74" t="s">
         <v>241</v>
       </c>
@@ -7430,8 +7430,8 @@
       <c r="N89" s="52"/>
     </row>
     <row r="90" spans="2:18" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="121"/>
-      <c r="C90" s="122"/>
+      <c r="B90" s="116"/>
+      <c r="C90" s="117"/>
       <c r="D90" s="74" t="s">
         <v>241</v>
       </c>
@@ -7467,8 +7467,8 @@
       <c r="N90" s="52"/>
     </row>
     <row r="91" spans="2:18" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B91" s="121"/>
-      <c r="C91" s="122"/>
+      <c r="B91" s="116"/>
+      <c r="C91" s="117"/>
       <c r="D91" s="74" t="s">
         <v>241</v>
       </c>
@@ -7504,8 +7504,8 @@
       <c r="N91" s="52"/>
     </row>
     <row r="92" spans="2:18" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B92" s="121"/>
-      <c r="C92" s="122"/>
+      <c r="B92" s="116"/>
+      <c r="C92" s="117"/>
       <c r="D92" s="74" t="s">
         <v>241</v>
       </c>
@@ -7541,8 +7541,8 @@
       <c r="N92" s="52"/>
     </row>
     <row r="93" spans="2:18" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B93" s="121"/>
-      <c r="C93" s="122"/>
+      <c r="B93" s="116"/>
+      <c r="C93" s="117"/>
       <c r="D93" s="74" t="s">
         <v>241</v>
       </c>
@@ -7578,8 +7578,8 @@
       <c r="N93" s="52"/>
     </row>
     <row r="94" spans="2:18" s="53" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B94" s="121"/>
-      <c r="C94" s="122"/>
+      <c r="B94" s="116"/>
+      <c r="C94" s="117"/>
       <c r="D94" s="74" t="s">
         <v>241</v>
       </c>
@@ -7615,8 +7615,8 @@
       <c r="N94" s="52"/>
     </row>
     <row r="95" spans="2:18" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B95" s="121"/>
-      <c r="C95" s="122"/>
+      <c r="B95" s="116"/>
+      <c r="C95" s="117"/>
       <c r="D95" s="74" t="s">
         <v>242</v>
       </c>
@@ -7674,10 +7674,10 @@
       </c>
     </row>
     <row r="97" spans="2:14" s="67" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B97" s="126" t="s">
+      <c r="B97" s="121" t="s">
         <v>176</v>
       </c>
-      <c r="C97" s="119" t="s">
+      <c r="C97" s="122" t="s">
         <v>232</v>
       </c>
       <c r="D97" s="74" t="s">
@@ -7709,8 +7709,8 @@
       <c r="N97" s="66"/>
     </row>
     <row r="98" spans="2:14" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B98" s="126"/>
-      <c r="C98" s="119"/>
+      <c r="B98" s="121"/>
+      <c r="C98" s="122"/>
       <c r="D98" s="74" t="s">
         <v>242</v>
       </c>
@@ -7740,8 +7740,8 @@
       <c r="N98" s="66"/>
     </row>
     <row r="99" spans="2:14" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B99" s="126"/>
-      <c r="C99" s="119"/>
+      <c r="B99" s="121"/>
+      <c r="C99" s="122"/>
       <c r="D99" s="74" t="s">
         <v>242</v>
       </c>
@@ -7771,8 +7771,8 @@
       <c r="N99" s="66"/>
     </row>
     <row r="100" spans="2:14" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B100" s="126"/>
-      <c r="C100" s="119"/>
+      <c r="B100" s="121"/>
+      <c r="C100" s="122"/>
       <c r="D100" s="74" t="s">
         <v>242</v>
       </c>
@@ -7802,8 +7802,8 @@
       <c r="N100" s="66"/>
     </row>
     <row r="101" spans="2:14" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B101" s="126"/>
-      <c r="C101" s="119"/>
+      <c r="B101" s="121"/>
+      <c r="C101" s="122"/>
       <c r="D101" s="74" t="s">
         <v>242</v>
       </c>
@@ -7833,8 +7833,8 @@
       <c r="N101" s="66"/>
     </row>
     <row r="102" spans="2:14" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B102" s="126"/>
-      <c r="C102" s="119"/>
+      <c r="B102" s="121"/>
+      <c r="C102" s="122"/>
       <c r="D102" s="74" t="s">
         <v>242</v>
       </c>
@@ -7864,8 +7864,8 @@
       <c r="N102" s="66"/>
     </row>
     <row r="103" spans="2:14" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B103" s="126"/>
-      <c r="C103" s="119"/>
+      <c r="B103" s="121"/>
+      <c r="C103" s="122"/>
       <c r="D103" s="74" t="s">
         <v>242</v>
       </c>
@@ -7895,8 +7895,8 @@
       <c r="N103" s="66"/>
     </row>
     <row r="104" spans="2:14" s="67" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B104" s="126"/>
-      <c r="C104" s="119"/>
+      <c r="B104" s="121"/>
+      <c r="C104" s="122"/>
       <c r="D104" s="74" t="s">
         <v>242</v>
       </c>
@@ -7926,8 +7926,8 @@
       <c r="N104" s="66"/>
     </row>
     <row r="105" spans="2:14" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B105" s="126"/>
-      <c r="C105" s="119"/>
+      <c r="B105" s="121"/>
+      <c r="C105" s="122"/>
       <c r="D105" s="74" t="s">
         <v>243</v>
       </c>
@@ -7957,8 +7957,8 @@
       <c r="N105" s="66"/>
     </row>
     <row r="106" spans="2:14" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B106" s="126"/>
-      <c r="C106" s="119"/>
+      <c r="B106" s="121"/>
+      <c r="C106" s="122"/>
       <c r="D106" s="74" t="s">
         <v>243</v>
       </c>
@@ -8758,76 +8758,101 @@
       <c r="C138" s="57" t="s">
         <v>232</v>
       </c>
-      <c r="D138" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="E138" s="46">
-        <v>0.95</v>
-      </c>
-      <c r="F138" s="46">
-        <v>0.95</v>
-      </c>
-      <c r="G138" s="46">
-        <v>0.95</v>
-      </c>
-      <c r="H138" s="46">
-        <v>0.95</v>
-      </c>
-      <c r="I138" s="46">
-        <v>0.95</v>
-      </c>
-      <c r="J138" s="46">
-        <v>0.95</v>
+      <c r="D138" s="78" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" s="7"/>
       <c r="C139" s="58"/>
-      <c r="D139" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="E139" s="46">
-        <v>0</v>
-      </c>
-      <c r="F139" s="46">
-        <v>0</v>
-      </c>
-      <c r="G139" s="46">
-        <v>0</v>
-      </c>
-      <c r="H139" s="46">
-        <v>0</v>
-      </c>
-      <c r="I139" s="46">
-        <v>0</v>
-      </c>
-      <c r="J139" s="46">
-        <v>0</v>
+      <c r="D139" s="34" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" s="7"/>
       <c r="C140" s="58"/>
-      <c r="D140" s="7" t="s">
+      <c r="D140" s="34" t="s">
+        <v>156</v>
+      </c>
+      <c r="E140" s="46">
+        <v>0.95</v>
+      </c>
+      <c r="F140" s="46">
+        <v>0.95</v>
+      </c>
+      <c r="G140" s="46">
+        <v>0.95</v>
+      </c>
+      <c r="H140" s="46">
+        <v>0.95</v>
+      </c>
+      <c r="I140" s="46">
+        <v>0.95</v>
+      </c>
+      <c r="J140" s="46">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D141" s="34" t="s">
+        <v>157</v>
+      </c>
+      <c r="E141" s="46">
+        <v>0</v>
+      </c>
+      <c r="F141" s="46">
+        <v>0</v>
+      </c>
+      <c r="G141" s="46">
+        <v>0</v>
+      </c>
+      <c r="H141" s="46">
+        <v>0</v>
+      </c>
+      <c r="I141" s="46">
+        <v>0</v>
+      </c>
+      <c r="J141" s="46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D142" s="34" t="s">
         <v>158</v>
       </c>
-      <c r="E140" s="46">
-        <v>0</v>
-      </c>
-      <c r="F140" s="46">
-        <v>0</v>
-      </c>
-      <c r="G140" s="46">
-        <v>0</v>
-      </c>
-      <c r="H140" s="46">
-        <v>0</v>
-      </c>
-      <c r="I140" s="46">
-        <v>0</v>
-      </c>
-      <c r="J140" s="46">
-        <v>0</v>
+      <c r="E142" s="46">
+        <v>0</v>
+      </c>
+      <c r="F142" s="46">
+        <v>0</v>
+      </c>
+      <c r="G142" s="46">
+        <v>0</v>
+      </c>
+      <c r="H142" s="46">
+        <v>0</v>
+      </c>
+      <c r="I142" s="46">
+        <v>0</v>
+      </c>
+      <c r="J142" s="46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D143" s="34" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D144" s="34" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="145" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D145" s="79" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="172" spans="2:10" x14ac:dyDescent="0.25">
@@ -8837,7 +8862,7 @@
       <c r="C172" s="73"/>
     </row>
     <row r="173" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C173" s="123" t="s">
+      <c r="C173" s="118" t="s">
         <v>232</v>
       </c>
       <c r="D173" s="7" t="s">
@@ -8863,7 +8888,7 @@
       </c>
     </row>
     <row r="174" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C174" s="124"/>
+      <c r="C174" s="119"/>
       <c r="D174" s="7" t="s">
         <v>157</v>
       </c>
@@ -8887,7 +8912,7 @@
       </c>
     </row>
     <row r="175" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C175" s="124"/>
+      <c r="C175" s="119"/>
       <c r="D175" s="7" t="s">
         <v>158</v>
       </c>
@@ -8912,6 +8937,13 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B8:B17"/>
+    <mergeCell ref="C8:C17"/>
+    <mergeCell ref="B19:B28"/>
+    <mergeCell ref="C19:C28"/>
+    <mergeCell ref="B75:B84"/>
+    <mergeCell ref="C75:C84"/>
+    <mergeCell ref="C63:C72"/>
     <mergeCell ref="B86:B95"/>
     <mergeCell ref="C86:C95"/>
     <mergeCell ref="C173:C175"/>
@@ -8924,13 +8956,6 @@
     <mergeCell ref="B63:B72"/>
     <mergeCell ref="B97:B106"/>
     <mergeCell ref="C97:C106"/>
-    <mergeCell ref="B8:B17"/>
-    <mergeCell ref="C8:C17"/>
-    <mergeCell ref="B19:B28"/>
-    <mergeCell ref="C19:C28"/>
-    <mergeCell ref="B75:B84"/>
-    <mergeCell ref="C75:C84"/>
-    <mergeCell ref="C63:C72"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="44" orientation="portrait" r:id="rId1"/>
@@ -8944,8 +8969,8 @@
   </sheetPr>
   <dimension ref="B1:N45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M33" sqref="M33"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9045,7 +9070,7 @@
       <c r="B6" s="115" t="s">
         <v>178</v>
       </c>
-      <c r="C6" s="123" t="s">
+      <c r="C6" s="118" t="s">
         <v>227</v>
       </c>
       <c r="D6" s="30" t="s">
@@ -9072,7 +9097,7 @@
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="115"/>
-      <c r="C7" s="124"/>
+      <c r="C7" s="119"/>
       <c r="D7" s="30" t="s">
         <v>155</v>
       </c>
@@ -9097,7 +9122,7 @@
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="115"/>
-      <c r="C8" s="124"/>
+      <c r="C8" s="119"/>
       <c r="D8" s="30" t="s">
         <v>156</v>
       </c>
@@ -9110,7 +9135,7 @@
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="115"/>
-      <c r="C9" s="124"/>
+      <c r="C9" s="119"/>
       <c r="D9" s="30" t="s">
         <v>157</v>
       </c>
@@ -9135,7 +9160,7 @@
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="115"/>
-      <c r="C10" s="124"/>
+      <c r="C10" s="119"/>
       <c r="D10" s="30" t="s">
         <v>158</v>
       </c>
@@ -9148,7 +9173,7 @@
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" s="115"/>
-      <c r="C11" s="124"/>
+      <c r="C11" s="119"/>
       <c r="D11" s="30" t="s">
         <v>159</v>
       </c>
@@ -9161,7 +9186,7 @@
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="115"/>
-      <c r="C12" s="124"/>
+      <c r="C12" s="119"/>
       <c r="D12" s="30" t="s">
         <v>160</v>
       </c>
@@ -9174,7 +9199,7 @@
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="115"/>
-      <c r="C13" s="124"/>
+      <c r="C13" s="119"/>
       <c r="D13" s="30" t="s">
         <v>166</v>
       </c>
@@ -9189,7 +9214,7 @@
       <c r="B15" s="115" t="s">
         <v>179</v>
       </c>
-      <c r="C15" s="123" t="s">
+      <c r="C15" s="118" t="s">
         <v>227</v>
       </c>
       <c r="D15" s="30" t="s">
@@ -9216,7 +9241,7 @@
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" s="115"/>
-      <c r="C16" s="124"/>
+      <c r="C16" s="119"/>
       <c r="D16" s="30" t="s">
         <v>155</v>
       </c>
@@ -9241,7 +9266,7 @@
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="115"/>
-      <c r="C17" s="124"/>
+      <c r="C17" s="119"/>
       <c r="D17" s="30" t="s">
         <v>156</v>
       </c>
@@ -9254,7 +9279,7 @@
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="115"/>
-      <c r="C18" s="124"/>
+      <c r="C18" s="119"/>
       <c r="D18" s="30" t="s">
         <v>157</v>
       </c>
@@ -9279,7 +9304,7 @@
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="115"/>
-      <c r="C19" s="124"/>
+      <c r="C19" s="119"/>
       <c r="D19" s="30" t="s">
         <v>158</v>
       </c>
@@ -9296,7 +9321,7 @@
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" s="115"/>
-      <c r="C20" s="124"/>
+      <c r="C20" s="119"/>
       <c r="D20" s="30" t="s">
         <v>159</v>
       </c>
@@ -9309,7 +9334,7 @@
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" s="115"/>
-      <c r="C21" s="124"/>
+      <c r="C21" s="119"/>
       <c r="D21" s="30" t="s">
         <v>160</v>
       </c>
@@ -9334,7 +9359,7 @@
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" s="115"/>
-      <c r="C22" s="124"/>
+      <c r="C22" s="119"/>
       <c r="D22" s="30" t="s">
         <v>166</v>
       </c>
@@ -9417,7 +9442,7 @@
       <c r="B27" s="115" t="s">
         <v>182</v>
       </c>
-      <c r="C27" s="123" t="s">
+      <c r="C27" s="118" t="s">
         <v>232</v>
       </c>
       <c r="D27" s="30" t="s">
@@ -9444,7 +9469,7 @@
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B28" s="115"/>
-      <c r="C28" s="124"/>
+      <c r="C28" s="119"/>
       <c r="D28" s="30" t="s">
         <v>155</v>
       </c>
@@ -9469,7 +9494,7 @@
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B29" s="115"/>
-      <c r="C29" s="124"/>
+      <c r="C29" s="119"/>
       <c r="D29" s="30" t="s">
         <v>156</v>
       </c>
@@ -9494,7 +9519,7 @@
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B30" s="115"/>
-      <c r="C30" s="124"/>
+      <c r="C30" s="119"/>
       <c r="D30" s="30" t="s">
         <v>157</v>
       </c>
@@ -9519,7 +9544,7 @@
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B31" s="115"/>
-      <c r="C31" s="124"/>
+      <c r="C31" s="119"/>
       <c r="D31" s="30" t="s">
         <v>158</v>
       </c>
@@ -9548,7 +9573,7 @@
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B32" s="115"/>
-      <c r="C32" s="124"/>
+      <c r="C32" s="119"/>
       <c r="D32" s="30" t="s">
         <v>159</v>
       </c>
@@ -9573,7 +9598,7 @@
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B33" s="115"/>
-      <c r="C33" s="124"/>
+      <c r="C33" s="119"/>
       <c r="D33" s="30" t="s">
         <v>160</v>
       </c>
@@ -9598,7 +9623,7 @@
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B34" s="115"/>
-      <c r="C34" s="124"/>
+      <c r="C34" s="119"/>
       <c r="D34" s="30" t="s">
         <v>166</v>
       </c>
@@ -9628,7 +9653,7 @@
       <c r="B38" s="115" t="s">
         <v>199</v>
       </c>
-      <c r="C38" s="123" t="s">
+      <c r="C38" s="118" t="s">
         <v>229</v>
       </c>
       <c r="D38" s="9" t="s">
@@ -9658,7 +9683,7 @@
     </row>
     <row r="39" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B39" s="115"/>
-      <c r="C39" s="124"/>
+      <c r="C39" s="119"/>
       <c r="D39" s="54">
         <v>25</v>
       </c>
@@ -9674,7 +9699,7 @@
     </row>
     <row r="40" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B40" s="115"/>
-      <c r="C40" s="124"/>
+      <c r="C40" s="119"/>
       <c r="D40" s="30"/>
       <c r="E40" s="26"/>
       <c r="F40" s="26"/>
@@ -9685,7 +9710,7 @@
     </row>
     <row r="41" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B41" s="115"/>
-      <c r="C41" s="124"/>
+      <c r="C41" s="119"/>
       <c r="D41" s="30"/>
       <c r="E41" s="26"/>
       <c r="F41" s="26"/>
@@ -9696,7 +9721,7 @@
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B42" s="115"/>
-      <c r="C42" s="124"/>
+      <c r="C42" s="119"/>
       <c r="D42" s="30"/>
       <c r="E42" s="26"/>
       <c r="F42" s="26"/>
@@ -9709,7 +9734,7 @@
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B43" s="115"/>
-      <c r="C43" s="124"/>
+      <c r="C43" s="119"/>
       <c r="D43" s="30"/>
       <c r="E43" s="26"/>
       <c r="F43" s="26"/>
@@ -9720,7 +9745,7 @@
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B44" s="115"/>
-      <c r="C44" s="124"/>
+      <c r="C44" s="119"/>
       <c r="D44" s="30"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
@@ -9731,7 +9756,7 @@
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B45" s="115"/>
-      <c r="C45" s="124"/>
+      <c r="C45" s="119"/>
       <c r="D45" s="30"/>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
@@ -17161,8 +17186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="L70" sqref="L70"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23:D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>